<commit_message>
obs solo con lp
</commit_message>
<xml_diff>
--- a/Docs/ISIS1225 - Tablas de Datos Lab 7.xlsx
+++ b/Docs/ISIS1225 - Tablas de Datos Lab 7.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Linds\Desktop\Liv-stuff\MAESTRIA\SEGUNDO SEMESTRE\ASISTENCIA\lab 7 JP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GMIPC\OneDrive - Universidad de los andes\Documentos\UNIVERSIDAD\UNIANDES\TERCER SEMESTRE\EDA\Lab 7\Laboratorio-7-G04\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73FE89C1-6036-4B20-A2C9-FA3316217E92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C828F3B-6581-47C3-B3F4-3742DE484C7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" tabRatio="767" xr2:uid="{D82936D8-D2C9-4EB2-9CBC-3665F65B95FD}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" tabRatio="767" xr2:uid="{D82936D8-D2C9-4EB2-9CBC-3665F65B95FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Datos Lab7" sheetId="1" r:id="rId1"/>
@@ -29,8 +29,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -137,7 +135,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -165,11 +163,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -189,9 +196,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -204,11 +208,26 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="7">
     <dxf>
       <font>
         <b val="0"/>
@@ -354,58 +373,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -455,7 +422,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -528,7 +495,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -615,7 +582,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="es-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -624,8 +591,20 @@
             <c:numRef>
               <c:f>'Datos Lab7'!$B$3:$B$6</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2210470.1460000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1820936.7109999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1712145.3459999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1593599.3859999999</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -633,8 +612,20 @@
             <c:numRef>
               <c:f>'Datos Lab7'!$C$3:$C$6</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>99410.392000000007</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>83507.486000000004</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>88886.338000000003</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>306333.31400000001</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -722,7 +713,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="es-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -835,11 +826,11 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -873,7 +864,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1087681551"/>
@@ -960,11 +951,11 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -998,7 +989,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1087686127"/>
@@ -1040,7 +1031,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1070,7 +1061,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-CO"/>
     </a:p>
   </c:txPr>
 </c:chartSpace>
@@ -1079,7 +1070,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1143,7 +1134,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1267,7 +1258,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="es-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -1297,8 +1288,20 @@
             <c:numRef>
               <c:f>'Datos Lab7'!$B$3:$B$6</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2210470.1460000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1820936.7109999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1712145.3459999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1593599.3859999999</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -1413,7 +1416,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="es-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -1533,7 +1536,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1568,7 +1571,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1086959919"/>
@@ -1641,11 +1644,11 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1675,7 +1678,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1086958255"/>
@@ -1714,7 +1717,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1744,7 +1747,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-CO"/>
     </a:p>
   </c:txPr>
 </c:chartSpace>
@@ -2823,7 +2826,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{CAFD5B44-21B9-42C7-B503-C146EF1BA3EE}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="78" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="70" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2834,7 +2837,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{680E7371-595A-4F03-ABE3-E0257A96E5F2}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="78" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="70" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2845,7 +2848,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8664087" cy="6276731"/>
+    <xdr:ext cx="8654143" cy="6277429"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -2878,7 +2881,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8664087" cy="6276731"/>
+    <xdr:ext cx="8654143" cy="6277429"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -2908,12 +2911,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{072D0253-75B0-4C0B-8972-D03303899249}" name="Table1" displayName="Table1" ref="A2:C6" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{072D0253-75B0-4C0B-8972-D03303899249}" name="Table1" displayName="Table1" ref="A2:C6" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
   <autoFilter ref="A2:C6" xr:uid="{B245DDE7-54F2-4A7A-AC17-5CA17DD7B03F}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{A7AF2A2F-BC4B-404E-9B8B-256DA178E68B}" name="Factor de Carga (PROBING)"/>
-    <tableColumn id="5" xr3:uid="{F280BCD9-1105-4F25-860B-4E27D28E75B2}" name="Consumo de Datos [kB]" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{23CECC62-35E0-466E-9502-4F5CC2E6F7A7}" name="Tiempo de Ejecución Real @LP [ms]" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{F280BCD9-1105-4F25-860B-4E27D28E75B2}" name="Consumo de Datos [kB]"/>
+    <tableColumn id="2" xr3:uid="{23CECC62-35E0-466E-9502-4F5CC2E6F7A7}" name="Tiempo de Ejecución Real @LP [ms]"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2932,9 +2935,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2972,7 +2975,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -3078,7 +3081,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -3220,7 +3223,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3231,24 +3234,24 @@
   <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11:C14"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="27.73046875" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.7265625" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.1328125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.08984375" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18" x14ac:dyDescent="0.45">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:3" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
     </row>
-    <row r="2" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -3259,42 +3262,58 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A3" s="8">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" s="7">
         <v>0.1</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="7"/>
+      <c r="B3" s="11">
+        <v>2210470.1460000002</v>
+      </c>
+      <c r="C3" s="12">
+        <v>99410.392000000007</v>
+      </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A4" s="9">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" s="8">
         <v>0.5</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="7"/>
+      <c r="B4" s="1">
+        <v>1820936.7109999999</v>
+      </c>
+      <c r="C4" s="13">
+        <v>83507.486000000004</v>
+      </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A5" s="8">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" s="7">
         <v>0.7</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="7"/>
+      <c r="B5" s="11">
+        <v>1712145.3459999999</v>
+      </c>
+      <c r="C5" s="12">
+        <v>88886.338000000003</v>
+      </c>
     </row>
-    <row r="6" spans="1:3" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A6" s="10">
+    <row r="6" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="9">
         <v>0.9</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="7"/>
+      <c r="B6" s="14">
+        <v>1593599.3859999999</v>
+      </c>
+      <c r="C6" s="15">
+        <v>306333.31400000001</v>
+      </c>
     </row>
-    <row r="9" spans="1:3" ht="18" x14ac:dyDescent="0.45">
-      <c r="A9" s="11" t="s">
+    <row r="9" spans="1:3" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="A9" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="11"/>
-      <c r="C9" s="11"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
     </row>
-    <row r="10" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>5</v>
       </c>
@@ -3305,35 +3324,35 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
         <v>2</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="5"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="2">
         <v>4</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="2">
         <v>6</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="2">
         <v>8</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
     </row>
-    <row r="23" ht="14.65" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="23" ht="14.65" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:C1"/>
@@ -3348,15 +3367,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x01010023858CF01A2EF24688B692775F4C60A4" ma:contentTypeVersion="17" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="af74a0f8eb440a60883e9dd833f0742f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="164883f8-7691-4ecf-b54a-664c0d0edefe" xmlns:ns3="85e30bcc-d76c-4413-8e4d-2dce22fb0743" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f5ceeff32ffca1089660572a8ebd1782" ns2:_="" ns3:_="">
     <xsd:import namespace="164883f8-7691-4ecf-b54a-664c0d0edefe"/>
@@ -3605,6 +3615,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -3617,14 +3636,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8DF3742-38F2-4B99-B335-CC4F04ED9F45}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E10B9E65-6C88-4633-81F7-F02338B2B10B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3643,6 +3654,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8DF3742-38F2-4B99-B335-CC4F04ED9F45}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97C5E1E0-C817-4769-9D2D-1DC296B681FA}">
   <ds:schemaRefs>

</xml_diff>